<commit_message>
add method to abort running script if three steps are continuous failed.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST962_AddDevice.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST962_AddDevice.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18195" windowHeight="9570"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="15480" windowHeight="9570"/>
   </bookViews>
   <sheets>
     <sheet name="Scripts" sheetId="3" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7787" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7787" uniqueCount="907">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4061,6 +4061,10 @@
   </si>
   <si>
     <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4582,7 +4586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -4736,7 +4742,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>842</v>
+        <v>906</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Move hard coded info to app.config
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST962_AddDevice.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST962_AddDevice.xlsx
@@ -1259,7 +1259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7787" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7789" uniqueCount="911">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -4073,6 +4073,14 @@
   </si>
   <si>
     <t>$SNMP_SearchEnd$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Running Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4595,7 +4603,7 @@
   <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4832,9 +4840,11 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>811</v>
-      </c>
-      <c r="B8" s="6"/>
+        <v>909</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>910</v>
+      </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
@@ -4862,11 +4872,9 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>820</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>821</v>
-      </c>
+        <v>811</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="3">
         <v>8</v>
       </c>
@@ -4891,8 +4899,12 @@
       <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>821</v>
+      </c>
       <c r="C10" s="3">
         <v>9</v>
       </c>
@@ -4917,10 +4929,8 @@
       <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="2" t="s">
-        <v>823</v>
-      </c>
-      <c r="B11" s="14"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="3">
         <v>10</v>
       </c>
@@ -4944,7 +4954,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="3">
@@ -4974,7 +4984,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="3">
@@ -5004,7 +5014,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="3">
@@ -5034,7 +5044,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="3">
@@ -5064,7 +5074,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="3">
@@ -5091,10 +5101,10 @@
       <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" ht="14.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="14" t="s">
-        <v>829</v>
-      </c>
+      <c r="A17" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B17" s="14"/>
       <c r="C17" s="3">
         <v>16</v>
       </c>
@@ -5121,7 +5131,7 @@
     <row r="18" spans="1:14" ht="14.25">
       <c r="A18" s="2"/>
       <c r="B18" s="14" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C18" s="3">
         <v>17</v>
@@ -5149,11 +5159,9 @@
       <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="2" t="s">
-        <v>831</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" s="14" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
       <c r="C19" s="3">
         <v>18</v>
@@ -5180,9 +5188,11 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="B20" s="14"/>
+        <v>831</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>821</v>
+      </c>
       <c r="C20" s="3">
         <v>19</v>
       </c>
@@ -5208,7 +5218,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B21" s="14"/>
       <c r="C21" s="3">
@@ -5235,6 +5245,10 @@
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="1:14">
+      <c r="A22" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B22" s="14"/>
       <c r="C22" s="3">
         <v>21</v>
       </c>

</xml_diff>